<commit_message>
To run in test machine
</commit_message>
<xml_diff>
--- a/testData/ExecuteTask/Notification/ETRS/ET_NT_ETRS_MTAfterDays_Test.xlsx
+++ b/testData/ExecuteTask/Notification/ETRS/ET_NT_ETRS_MTAfterDays_Test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="80">
   <si>
     <t>ModuleName</t>
   </si>
@@ -171,9 +171,6 @@
     <t>NotifyTemplate_Msg</t>
   </si>
   <si>
-    <t xml:space="preserve"> ET_OOFS_Notify </t>
-  </si>
-  <si>
     <t>RelatedModuleText</t>
   </si>
   <si>
@@ -255,29 +252,22 @@
     <t>05-24-2024 05:00:00 PM</t>
   </si>
   <si>
-    <t>ET348</t>
-  </si>
-  <si>
-    <t>ET350</t>
-  </si>
-  <si>
     <t>tskNT_ExecuteTask_MTAfterDays</t>
   </si>
   <si>
-    <t>ET351</t>
-  </si>
-  <si>
     <t>ET354</t>
   </si>
   <si>
     <t>ET356</t>
+  </si>
+  <si>
+    <t>ET_ETRS_Notify</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -626,38 +616,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AF2" sqref="AF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="13.26953125"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.0"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="11.1796875"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="12.54296875"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="14.7265625"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="20.0"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="12.54296875"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="11.1796875"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="16.81640625"/>
-    <col min="10" max="17" style="1" width="9.1796875"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="11.0"/>
-    <col min="19" max="19" style="1" width="9.1796875"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="23.0"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="8.0"/>
-    <col min="22" max="23" style="1" width="9.1796875"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="18.81640625"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="20.0"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="16.26953125"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="33.54296875"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="8.81640625"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="12.81640625"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="20.0"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="11.0"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="19.81640625"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="12.26953125"/>
-    <col min="34" max="16384" style="1" width="9.1796875"/>
+    <col min="1" max="1" width="13.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="17" width="9.1796875" style="1"/>
+    <col min="18" max="18" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.1796875" style="1"/>
+    <col min="20" max="20" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="9.1796875" style="1"/>
+    <col min="24" max="24" width="18.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="33.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.35">
@@ -758,7 +748,7 @@
         <v>48</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.35">
@@ -766,7 +756,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>25</v>
@@ -792,8 +782,8 @@
       <c r="J2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K2" t="s" s="1">
-        <v>75</v>
+      <c r="K2" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="L2" s="1">
         <v>1</v>
@@ -801,11 +791,11 @@
       <c r="M2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N2" t="s" s="1">
-        <v>76</v>
-      </c>
-      <c r="O2" t="s" s="1">
-        <v>69</v>
+      <c r="N2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>33</v>
@@ -820,7 +810,7 @@
         <v>1000</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="U2" s="1" t="s">
         <v>35</v>
@@ -832,16 +822,16 @@
         <v>37</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Z2" s="1" t="s">
         <v>41</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="AB2" s="1" t="s">
         <v>44</v>
@@ -853,13 +843,13 @@
         <v>47</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AG2" t="s" s="1">
-        <v>81</v>
-      </c>
-      <c r="AK2" t="s" s="1">
-        <v>74</v>
+        <v>79</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -875,29 +865,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2"/>
+    <sheetView topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AF2" sqref="AF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.7265625"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="25.0"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.7265625"/>
-    <col min="6" max="6" customWidth="true" width="21.453125"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.54296875"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="16.81640625"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="11.81640625"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="21.7265625"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="11.453125"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="11.0"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="23.81640625"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="20.0"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="16.26953125"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="33.54296875"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="19.81640625"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="11.0"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="19.81640625"/>
+    <col min="1" max="1" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.453125" customWidth="1"/>
+    <col min="7" max="7" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="33.54296875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.35">
@@ -998,7 +988,7 @@
         <v>48</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.35">
@@ -1006,7 +996,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>25</v>
@@ -1018,22 +1008,22 @@
         <v>1234567890</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K2" t="s" s="0">
-        <v>75</v>
+      <c r="K2" t="s">
+        <v>74</v>
       </c>
       <c r="L2" s="1">
         <v>1</v>
@@ -1041,17 +1031,17 @@
       <c r="M2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N2" t="s" s="0">
-        <v>76</v>
-      </c>
-      <c r="O2" t="s" s="0">
-        <v>69</v>
+      <c r="N2" t="s">
+        <v>75</v>
+      </c>
+      <c r="O2" t="s">
+        <v>68</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="R2" s="1">
         <v>2323232323</v>
@@ -1060,10 +1050,10 @@
         <v>1000</v>
       </c>
       <c r="T2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="V2" s="1" t="s">
         <v>36</v>
@@ -1072,16 +1062,16 @@
         <v>37</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Z2" s="1" t="s">
         <v>41</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
@@ -1092,10 +1082,10 @@
         <v>1199223344</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AG2" t="s" s="0">
-        <v>70</v>
+        <v>79</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1111,18 +1101,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="AA2" sqref="AA2"/>
+    <sheetView topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AF2" sqref="AF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.7265625"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="25.0"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.7265625"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="24.26953125"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="16.81640625"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.1796875"/>
+    <col min="1" max="1" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.35">
@@ -1223,15 +1213,15 @@
         <v>48</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:33" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>25</v>
@@ -1243,22 +1233,22 @@
         <v>1234567890</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K2" t="s" s="0">
-        <v>75</v>
+      <c r="K2" t="s">
+        <v>74</v>
       </c>
       <c r="L2" s="1">
         <v>1</v>
@@ -1266,17 +1256,17 @@
       <c r="M2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N2" t="s" s="0">
-        <v>76</v>
-      </c>
-      <c r="O2" t="s" s="0">
-        <v>69</v>
+      <c r="N2" t="s">
+        <v>75</v>
+      </c>
+      <c r="O2" t="s">
+        <v>68</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="R2" s="1">
         <v>2323232323</v>
@@ -1285,10 +1275,10 @@
         <v>1000</v>
       </c>
       <c r="T2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="V2" s="1" t="s">
         <v>36</v>
@@ -1297,16 +1287,16 @@
         <v>37</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Z2" s="1" t="s">
         <v>41</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
@@ -1317,10 +1307,10 @@
         <v>1199223344</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AG2" t="s" s="0">
-        <v>71</v>
+        <v>79</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1336,18 +1326,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AA3" sqref="AA3"/>
+    <sheetView topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AF2" sqref="AF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="25.0"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.1796875"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.7265625"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="24.453125"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="16.1796875"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="11.90625"/>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.35">
@@ -1448,15 +1438,15 @@
         <v>48</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:33" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>25</v>
@@ -1468,22 +1458,22 @@
         <v>1234567890</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>29</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K2" t="s" s="0">
-        <v>75</v>
+      <c r="K2" t="s">
+        <v>74</v>
       </c>
       <c r="L2" s="1">
         <v>1</v>
@@ -1491,17 +1481,17 @@
       <c r="M2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N2" t="s" s="0">
-        <v>76</v>
-      </c>
-      <c r="O2" t="s" s="0">
-        <v>69</v>
+      <c r="N2" t="s">
+        <v>75</v>
+      </c>
+      <c r="O2" t="s">
+        <v>68</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R2" s="1">
         <v>2323232323</v>
@@ -1510,10 +1500,10 @@
         <v>1000</v>
       </c>
       <c r="T2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="V2" s="1" t="s">
         <v>36</v>
@@ -1522,16 +1512,16 @@
         <v>37</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Z2" s="6" t="s">
         <v>41</v>
       </c>
       <c r="AA2" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
@@ -1542,10 +1532,10 @@
         <v>1199223344</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AG2" t="s" s="0">
-        <v>82</v>
+        <v>79</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>